<commit_message>
Unify version to v1118.6 across all files + update Excel guides
VERSION UNIFICATION:
- Updated update_excel_guides.py: 1118.4 → 1118.6
- Updated WIKI_CONFLUENCE.md: 1118.3 → 1118.6
- Updated Excel guides (EN/KR) to v1118.6 with dict fix changelog
- All files now consistent at v1118.6

EXCEL GUIDES UPDATED:
- Added v1118.6 changelog: Dict error fixes, comprehensive testing
- Korean translation added
- Script executed: python3 update_excel_guides.py

CLAUDE.MD UPDATED:
- Added version unification checklist
- Added update_excel_guides.py usage
- Added roadmap.md reference (project bible)
- Added fresh Claude setup guide
- Concise, essential info only

FILES NOW AT v1118.6:
✓ src/config.py
✓ main.py
✓ README.md
✓ README_KR.md
✓ roadmap.md
✓ update_excel_guides.py
✓ WIKI_CONFLUENCE.md
✓ VRS_Manager_Process_Guide_EN.xlsx
✓ VRS_Manager_Process_Guide_KR.xlsx

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/VRS_Manager_Process_Guide_EN.xlsx
+++ b/VRS_Manager_Process_Guide_EN.xlsx
@@ -586,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,7 +611,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 1118.4 (Enhanced Super Group Word Analysis)</t>
+          <t>Version 1118.6 (Dict Error Fixes + Comprehensive Testing)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -1748,6 +1748,177 @@
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
+        </is>
+      </c>
+    </row>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185">
+      <c r="A185" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v1118.6?</t>
+        </is>
+      </c>
+    </row>
+    <row r="186"/>
+    <row r="187">
+      <c r="A187" s="9" t="inlineStr">
+        <is>
+          <t>✅ Critical Bug Fixes (v1118.6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: TypeError 'unhashable type: dict' in Working VRS Check</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: All DataFrame column access now uses safe_str() pattern</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: Lookup dictionaries now correctly store indices (not dict objects)</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: 100% accuracy verified with 5000-row comprehensive test suite</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: All processors (Raw, Working, All Language) passing with real data</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="9" t="inlineStr">
+        <is>
+          <t>✅ Enhanced Super Group Word Analysis (v1118.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: 'Other' super group - Contains: Police, Minigame, Trade, Church, Shop, Contribution, RoyalSupply, Research, Quest Groups, faction_etc</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • RENAMED: Catch-all 'Other' → 'Everything Else' (for better clarity)</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Translation % (Previous) - Track translation progress from previous version</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Translation % Change - See translation progress difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Renamed: 'Untranslated Words' → 'Untranslated Words (Remaining to Translate)'</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Reorganized columns: Most important metrics first, related data grouped together</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Added explanatory note below table describing 'Everything Else'</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="9" t="inlineStr">
+        <is>
+          <t>Column Order (Reorganized for Better Readability):</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 1. Super Group Name, Total Words (Current/Previous), Net Change, % Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 2. Translated/Untranslated words, Translation % (Current/Previous/Change)</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 3. Detailed breakdown: Words Added/Deleted/Changed/Unchanged/Migrated</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame Preservation Restored</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame ONLY (EndFrame always updates from SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed AND StrOrigin changed → Update StartFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed BUT StrOrigin NOT changed → Preserve StartFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
         </is>
@@ -4937,7 +5108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6347,6 +6518,45 @@
     <row r="195"/>
     <row r="196">
       <c r="A196" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199">
+      <c r="A199" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="200"/>
+    <row r="201">
+      <c r="A201" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="204"/>
+    <row r="205">
+      <c r="A205" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>

<commit_message>
Comprehensive documentation update: Phase 2.2.1 completion
- Updated Excel guides (EN/KR) with comprehensive Phase 2.2.1 features
- Marked Phase 2.2.1 as COMPLETED in roadmap.md
- Updated all 16 implementation steps to [x] completed
- Added Phase 2.2.1 details to v1118.4 version history
- Enhanced update_excel_guides.py with full Phase 2.2.1 changelog

Phase 2.2.1 accomplishments:
- Removed "Others" super group and stageclosedialog check
- Reordered super groups: AI Dialog before Quest Dialog
- Renamed column header to "Not Translated"
- Removed migration columns from main table
- Added detailed "Super Group Migrations" table

🤖 Generated with Claude Code
</commit_message>
<xml_diff>
--- a/VRS_Manager_Process_Guide_EN.xlsx
+++ b/VRS_Manager_Process_Guide_EN.xlsx
@@ -586,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1919,6 +1919,184 @@
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
+        </is>
+      </c>
+    </row>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212">
+      <c r="A212" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v1118.6?</t>
+        </is>
+      </c>
+    </row>
+    <row r="213"/>
+    <row r="214">
+      <c r="A214" s="9" t="inlineStr">
+        <is>
+          <t>✅ Critical Bug Fixes (v1118.6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: TypeError 'unhashable type: dict' in Working VRS Check</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: All DataFrame column access now uses safe_str() pattern</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: Lookup dictionaries now correctly store indices (not dict objects)</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: 100% accuracy verified with 5000-row comprehensive test suite</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: All processors (Raw, Working, All Language) passing with real data</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 2.2.1 COMPLETED - Super Group Analysis Improvements (v1118.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: 'Others' super group and stageclosedialog check entirely</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REORDERED: Super groups - AI Dialog now appears before Quest Dialog</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • RENAMED: 'Untranslated Words (Remaining to Translate)' → 'Not Translated'</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: Migration columns from main table (Words Migrated In/Out)</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • ADDED: Detailed 'Super Group Migrations' table below main table</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows source → destination pairs with word counts for all migrations</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • UPDATED: Explanatory notes below table (removed 'Others' references)</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 8 super groups total: Main Chapters, F1, F2, F3, AI Dialog, Quest Dialog, Other, Everything Else</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="9" t="inlineStr">
+        <is>
+          <t>Column Order (Reorganized for Better Readability):</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 1. Super Group Name, Total Words (Current/Previous), Net Change, % Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 2. Translated/Untranslated words, Translation % (Current/Previous/Change)</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 3. Detailed breakdown: Words Added/Deleted/Changed/Unchanged/Migrated</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame Preservation Restored</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame ONLY (EndFrame always updates from SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed AND StrOrigin changed → Update StartFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed BUT StrOrigin NOT changed → Preserve StartFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
         </is>
@@ -5108,7 +5286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6557,6 +6735,45 @@
     <row r="204"/>
     <row r="205">
       <c r="A205" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208">
+      <c r="A208" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="209"/>
+    <row r="210">
+      <c r="A210" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="213"/>
+    <row r="214">
+      <c r="A214" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>